<commit_message>
Add 5 issue in Management
</commit_message>
<xml_diff>
--- a/Project Plan/[PIM]Reflection.xlsx
+++ b/Project Plan/[PIM]Reflection.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Difficulties</t>
   </si>
@@ -82,6 +82,51 @@
   </si>
   <si>
     <t>Asking the mentor and the internet for the solution in architect to give the good archiectect. Besides, explaning about the architect and dealing with design team are necessary</t>
+  </si>
+  <si>
+    <t>Member don’t care about Risks in project and don’t update Risk Category</t>
+  </si>
+  <si>
+    <t>Too much and more difficult to measurement</t>
+  </si>
+  <si>
+    <t>Project difficult to control and monitoring</t>
+  </si>
+  <si>
+    <t>Follow risk plan, plan about interation for risk</t>
+  </si>
+  <si>
+    <t>Knowing more about manage risk better</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Research about measurement, implement Goal-Question-Metric</t>
+  </si>
+  <si>
+    <t>Knowing more defenite about metrics and how to get it</t>
+  </si>
+  <si>
+    <t>Plan for detail plan, WBS, implement tracking and monitoring through measurement about schedule devition metric</t>
+  </si>
+  <si>
+    <t>Require team member write reflection base on 360 reivew</t>
+  </si>
+  <si>
+    <t>Knowing about management and communicate between team member</t>
+  </si>
+  <si>
+    <t>360 review is not good conduct</t>
+  </si>
+  <si>
+    <t>Team member is not complete work on time</t>
+  </si>
+  <si>
+    <t>Re-estimate, and evaluate effort of team member</t>
+  </si>
+  <si>
+    <t>Conduct measurement about productivity</t>
   </si>
 </sst>
 </file>
@@ -172,12 +217,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -186,6 +227,17 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,212 +542,274 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.42578125" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="6"/>
+    <col min="2" max="2" width="53.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="38.28515625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="A15" s="3">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="A17" s="3">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -707,7 +821,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>